<commit_message>
ajout descri, View Name
</commit_message>
<xml_diff>
--- a/excel/DATA_MIG.xlsx
+++ b/excel/DATA_MIG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AndrainaNyAinaRakoto\Documents\Bot ADR\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A5659E-B8E6-4454-94AE-D3A84CA7462D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8186F044-A952-4E61-81AB-2E3444B309E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6D3B04EF-C702-431C-B8A8-55B77D33493B}"/>
   </bookViews>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID job migration</t>
-  </si>
-  <si>
-    <t>Group job migration</t>
   </si>
   <si>
     <t>IWF_DATA_MIG</t>
@@ -613,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89B43582-F16E-4498-A06D-55666FFE6302}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -625,71 +622,66 @@
     <col min="2" max="2" width="160.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="11" t="s">
+      <c r="B2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>1</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>12</v>
-      </c>
       <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="9"/>
+      <c r="E5" s="9"/>
     </row>
     <row r="18" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="70" ht="28.8" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>